<commit_message>
deep dive on European-Native violence vs intra-European violence though topic models computed against page-chunked text
</commit_message>
<xml_diff>
--- a/mallet/10_AM.xlsx
+++ b/mallet/10_AM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apovzner\Documents\Hakluyt\mallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC4ACC4-12B9-43E1-B245-B3E55035353A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B828992-404D-45CB-8035-1239D2C8ECDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26970" windowHeight="10695" tabRatio="631" xr2:uid="{468B4E7C-0EDA-419C-AC8A-BFE265156530}"/>
   </bookViews>
@@ -692,12 +692,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -712,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -721,6 +727,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,12 +1044,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755A0F22-9D7C-42BD-B5D6-308444EEE854}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
@@ -1090,31 +1099,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>0.25983000000000001</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>0.29937999999999998</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1132,31 +1141,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>3.3610000000000001E-2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>0.18607000000000001</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>